<commit_message>
Added data for reverse for loop correlated mixed error as well as figures
</commit_message>
<xml_diff>
--- a/testData/transformTestData.xlsx
+++ b/testData/transformTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valde\OneDrive\Skrivebord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Desktop\Github\ESD5-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA70867A-56BA-4610-94AC-84C642A71E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB49AB7-7FA4-4576-AC09-67D9DCB1C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53243543-98D6-4300-B2A5-3A961808EFFC}"/>
+    <workbookView xWindow="11200" yWindow="0" windowWidth="11200" windowHeight="13400" xr2:uid="{53243543-98D6-4300-B2A5-3A961808EFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="80">
   <si>
     <t>ampUni01</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>combCor20-10-80</t>
+  </si>
+  <si>
+    <t>Reverse</t>
   </si>
 </sst>
 </file>
@@ -330,10 +333,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,22 +654,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FA19A4-6E8B-4763-B9A8-45A697D13A3C}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="N16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -729,7 +728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -806,7 +805,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -884,7 +883,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -962,7 +961,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1039,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1277,7 +1276,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1286,7 +1285,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1845,7 +1844,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1876,7 +1875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2353,7 +2352,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2433,7 +2432,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2521,7 +2520,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2604,8 +2603,11 @@
       <c r="O29" s="1">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2656,8 +2658,33 @@
       <c r="O30" s="1">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>70</v>
+      </c>
+      <c r="R30" s="2">
+        <f>0.001241</f>
+        <v>1.2409999999999999E-3</v>
+      </c>
+      <c r="S30" s="2">
+        <f>0.00024</f>
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="T30" s="2">
+        <f>0.002804</f>
+        <v>2.8040000000000001E-3</v>
+      </c>
+      <c r="U30" s="2">
+        <f>0.000382</f>
+        <v>3.8200000000000002E-4</v>
+      </c>
+      <c r="V30" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W30" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2707,8 +2734,33 @@
       <c r="O31" s="1">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>72</v>
+      </c>
+      <c r="R31" s="2">
+        <f>0.004597</f>
+        <v>4.5970000000000004E-3</v>
+      </c>
+      <c r="S31" s="2">
+        <f>0.000591</f>
+        <v>5.9100000000000005E-4</v>
+      </c>
+      <c r="T31" s="2">
+        <f>0.0056925</f>
+        <v>5.6924999999999996E-3</v>
+      </c>
+      <c r="U31" s="2">
+        <f>0.000937</f>
+        <v>9.3700000000000001E-4</v>
+      </c>
+      <c r="V31" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W31" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2759,8 +2811,33 @@
       <c r="O32" s="1">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>73</v>
+      </c>
+      <c r="R32" s="2">
+        <f>0.020387</f>
+        <v>2.0386999999999999E-2</v>
+      </c>
+      <c r="S32" s="2">
+        <f>0.003345</f>
+        <v>3.3449999999999999E-3</v>
+      </c>
+      <c r="T32" s="2">
+        <f>0.0202259</f>
+        <v>2.0225900000000002E-2</v>
+      </c>
+      <c r="U32" s="2">
+        <f>0.003955</f>
+        <v>3.9550000000000002E-3</v>
+      </c>
+      <c r="V32" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W32" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2810,8 +2887,33 @@
         <f>8+8.4</f>
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>71</v>
+      </c>
+      <c r="R33" s="2">
+        <f>0.00729</f>
+        <v>7.2899999999999996E-3</v>
+      </c>
+      <c r="S33" s="2">
+        <f>0.000763</f>
+        <v>7.6300000000000001E-4</v>
+      </c>
+      <c r="T33" s="2">
+        <f>0.004452</f>
+        <v>4.4520000000000002E-3</v>
+      </c>
+      <c r="U33" s="2">
+        <f>0.000855</f>
+        <v>8.5499999999999997E-4</v>
+      </c>
+      <c r="V33" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W33" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2861,8 +2963,33 @@
       <c r="O34" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34" t="s">
+        <v>77</v>
+      </c>
+      <c r="R34" s="2">
+        <f>0.018032</f>
+        <v>1.8031999999999999E-2</v>
+      </c>
+      <c r="S34" s="2">
+        <f>0.002525</f>
+        <v>2.5249999999999999E-3</v>
+      </c>
+      <c r="T34" s="2">
+        <f>0.016333</f>
+        <v>1.6333E-2</v>
+      </c>
+      <c r="U34" s="2">
+        <f>0.002822</f>
+        <v>2.8219999999999999E-3</v>
+      </c>
+      <c r="V34" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W34" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2888,8 +3015,33 @@
         <v>26.1</v>
       </c>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35" t="s">
+        <v>74</v>
+      </c>
+      <c r="R35" s="2">
+        <f>0.07073</f>
+        <v>7.0730000000000001E-2</v>
+      </c>
+      <c r="S35" s="2">
+        <f>0.0048049</f>
+        <v>4.8049E-3</v>
+      </c>
+      <c r="T35" s="2">
+        <f>0.0814612</f>
+        <v>8.1461199999999998E-2</v>
+      </c>
+      <c r="U35" s="2">
+        <f>0.01626</f>
+        <v>1.626E-2</v>
+      </c>
+      <c r="V35" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W35" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2922,8 +3074,33 @@
       <c r="O36" s="1">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36" t="s">
+        <v>75</v>
+      </c>
+      <c r="R36" s="2">
+        <f>0.005183</f>
+        <v>5.1830000000000001E-3</v>
+      </c>
+      <c r="S36" s="2">
+        <f>0.00066</f>
+        <v>6.6E-4</v>
+      </c>
+      <c r="T36" s="2">
+        <f>0.006492</f>
+        <v>6.4920000000000004E-3</v>
+      </c>
+      <c r="U36" s="2">
+        <f>0.001321</f>
+        <v>1.3209999999999999E-3</v>
+      </c>
+      <c r="V36" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W36" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -2953,8 +3130,33 @@
       <c r="O37" s="1">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>78</v>
+      </c>
+      <c r="R37" s="2">
+        <f>0.0294189</f>
+        <v>2.9418900000000001E-2</v>
+      </c>
+      <c r="S37" s="2">
+        <f>0.003344</f>
+        <v>3.3440000000000002E-3</v>
+      </c>
+      <c r="T37" s="2">
+        <f>0.019294</f>
+        <v>1.9293999999999999E-2</v>
+      </c>
+      <c r="U37" s="2">
+        <f>0.004577</f>
+        <v>4.5770000000000003E-3</v>
+      </c>
+      <c r="V37" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="W37" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -3005,8 +3207,34 @@
       <c r="O38" s="1">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38" t="s">
+        <v>76</v>
+      </c>
+      <c r="R38" s="2">
+        <f>0.067295</f>
+        <v>6.7294999999999994E-2</v>
+      </c>
+      <c r="S38" s="2">
+        <f>0.011521</f>
+        <v>1.1521E-2</v>
+      </c>
+      <c r="T38" s="2">
+        <f>0.118434</f>
+        <v>0.118434</v>
+      </c>
+      <c r="U38" s="2">
+        <f>0.024033</f>
+        <v>2.4032999999999999E-2</v>
+      </c>
+      <c r="V38" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="W38" s="1">
+        <f>12.4+14.2</f>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3058,7 +3286,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -3110,7 +3338,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3162,7 +3390,7 @@
         <v>26.3</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -3214,7 +3442,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -3266,7 +3494,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3323,12 +3551,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3482,15 +3707,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5C7046A-D9FD-4091-BEF8-46967EC5E81E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC555542-73CF-4BDB-AC57-32AF5F06904D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3514,17 +3750,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC555542-73CF-4BDB-AC57-32AF5F06904D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5C7046A-D9FD-4091-BEF8-46967EC5E81E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added figures and data for reversed order correlated error. Be wary, that the figures for phase are labeled incorrectly.
</commit_message>
<xml_diff>
--- a/testData/transformTestData.xlsx
+++ b/testData/transformTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Desktop\Github\ESD5-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB49AB7-7FA4-4576-AC09-67D9DCB1C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B8CE54-CA7D-42AB-8A92-3B20AF1B2EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="0" windowWidth="11200" windowHeight="13400" xr2:uid="{53243543-98D6-4300-B2A5-3A961808EFFC}"/>
+    <workbookView xWindow="12870" yWindow="0" windowWidth="9530" windowHeight="13400" xr2:uid="{53243543-98D6-4300-B2A5-3A961808EFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
   <si>
     <t>ampUni01</t>
   </si>
@@ -652,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FA19A4-6E8B-4763-B9A8-45A697D13A3C}">
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3545,18 +3545,487 @@
         <v>27</v>
       </c>
     </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="I46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="2">
+        <f>0.002074</f>
+        <v>2.0739999999999999E-3</v>
+      </c>
+      <c r="C47" s="2">
+        <f>0.0001839</f>
+        <v>1.839E-4</v>
+      </c>
+      <c r="D47" s="2">
+        <f>0.0013556</f>
+        <v>1.3556E-3</v>
+      </c>
+      <c r="E47" s="2">
+        <f>0.0002636</f>
+        <v>2.6360000000000001E-4</v>
+      </c>
+      <c r="F47" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G47" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I47" t="s">
+        <v>45</v>
+      </c>
+      <c r="J47" s="2">
+        <f>0.001101</f>
+        <v>1.101E-3</v>
+      </c>
+      <c r="K47" s="2">
+        <f>0.000148</f>
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="L47" s="2">
+        <f>0.000847</f>
+        <v>8.4699999999999999E-4</v>
+      </c>
+      <c r="M47" s="2">
+        <f>0.0002</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N47" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O47" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="2">
+        <f>0.003531</f>
+        <v>3.5309999999999999E-3</v>
+      </c>
+      <c r="C48" s="2">
+        <f>0.002811</f>
+        <v>2.8110000000000001E-3</v>
+      </c>
+      <c r="D48" s="2">
+        <f>0.00487</f>
+        <v>4.8700000000000002E-3</v>
+      </c>
+      <c r="E48" s="2">
+        <f>0.0036596</f>
+        <v>3.6595999999999998E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G48" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" s="2">
+        <f>0.001719</f>
+        <v>1.719E-3</v>
+      </c>
+      <c r="K48" s="2">
+        <f>0.000286</f>
+        <v>2.8600000000000001E-4</v>
+      </c>
+      <c r="L48" s="2">
+        <f>0.002531</f>
+        <v>2.5309999999999998E-3</v>
+      </c>
+      <c r="M48" s="2">
+        <f>0.000432</f>
+        <v>4.3199999999999998E-4</v>
+      </c>
+      <c r="N48" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O48" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="2">
+        <f>0.024789</f>
+        <v>2.4788999999999999E-2</v>
+      </c>
+      <c r="C49" s="2">
+        <f>0.00357</f>
+        <v>3.5699999999999998E-3</v>
+      </c>
+      <c r="D49" s="2">
+        <f>0.0358055</f>
+        <v>3.5805499999999997E-2</v>
+      </c>
+      <c r="E49" s="2">
+        <f>0.005808</f>
+        <v>5.8079999999999998E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G49" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I49" t="s">
+        <v>47</v>
+      </c>
+      <c r="J49" s="2">
+        <f>0.004048</f>
+        <v>4.0480000000000004E-3</v>
+      </c>
+      <c r="K49" s="2">
+        <f>0.000817</f>
+        <v>8.1700000000000002E-4</v>
+      </c>
+      <c r="L49" s="2">
+        <f>0.010917</f>
+        <v>1.0917E-2</v>
+      </c>
+      <c r="M49" s="2">
+        <f>0.00201</f>
+        <v>2.0100000000000001E-3</v>
+      </c>
+      <c r="N49" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O49" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="2">
+        <f>0.004385</f>
+        <v>4.385E-3</v>
+      </c>
+      <c r="C50" s="2">
+        <f>0.000526</f>
+        <v>5.2599999999999999E-4</v>
+      </c>
+      <c r="D50" s="2">
+        <f>0.002839</f>
+        <v>2.8389999999999999E-3</v>
+      </c>
+      <c r="E50" s="2">
+        <f>0.0007337</f>
+        <v>7.337E-4</v>
+      </c>
+      <c r="F50" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" s="2">
+        <f>0.00225</f>
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="K50" s="2">
+        <f>0.000318</f>
+        <v>3.1799999999999998E-4</v>
+      </c>
+      <c r="L50" s="2">
+        <f>0.002335</f>
+        <v>2.3349999999999998E-3</v>
+      </c>
+      <c r="M50" s="2">
+        <f>0.000453</f>
+        <v>4.5300000000000001E-4</v>
+      </c>
+      <c r="N50" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O50" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="2">
+        <f>0.0066254</f>
+        <v>6.6254E-3</v>
+      </c>
+      <c r="C51" s="2">
+        <f>0.001344</f>
+        <v>1.3439999999999999E-3</v>
+      </c>
+      <c r="D51" s="2">
+        <f>0.01331</f>
+        <v>1.3310000000000001E-2</v>
+      </c>
+      <c r="E51" s="2">
+        <f>0.0029</f>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G51" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I51" t="s">
+        <v>49</v>
+      </c>
+      <c r="J51" s="2">
+        <f>0.0069554</f>
+        <v>6.9553999999999996E-3</v>
+      </c>
+      <c r="K51" s="2">
+        <v>8.1700000000000002E-4</v>
+      </c>
+      <c r="L51" s="2">
+        <f>0.009103</f>
+        <v>9.103E-3</v>
+      </c>
+      <c r="M51" s="2">
+        <f>0.001305</f>
+        <v>1.305E-3</v>
+      </c>
+      <c r="N51" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O51" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="2">
+        <f>0.055519</f>
+        <v>5.5518999999999999E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <f>0.007414</f>
+        <v>7.4139999999999996E-3</v>
+      </c>
+      <c r="D52" s="2">
+        <f>0.0447646</f>
+        <v>4.4764600000000002E-2</v>
+      </c>
+      <c r="E52" s="2">
+        <f>0.010967</f>
+        <v>1.0966999999999999E-2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="G52" s="1">
+        <v>26.4</v>
+      </c>
+      <c r="I52" t="s">
+        <v>50</v>
+      </c>
+      <c r="J52" s="2">
+        <f>0.022773</f>
+        <v>2.2773000000000002E-2</v>
+      </c>
+      <c r="K52" s="2">
+        <f>0.003679</f>
+        <v>3.679E-3</v>
+      </c>
+      <c r="L52" s="2">
+        <f>0.026404</f>
+        <v>2.6404E-2</v>
+      </c>
+      <c r="M52" s="2">
+        <f>0.004405</f>
+        <v>4.4050000000000001E-3</v>
+      </c>
+      <c r="N52" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O52" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="2">
+        <f>0.0030116</f>
+        <v>3.0116000000000001E-3</v>
+      </c>
+      <c r="C53" s="2">
+        <f>0.000713</f>
+        <v>7.1299999999999998E-4</v>
+      </c>
+      <c r="D53" s="2">
+        <f>0.00398</f>
+        <v>3.98E-3</v>
+      </c>
+      <c r="E53" s="2">
+        <f>0.000857</f>
+        <v>8.5700000000000001E-4</v>
+      </c>
+      <c r="F53" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G53" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I53" t="s">
+        <v>51</v>
+      </c>
+      <c r="J53" s="2">
+        <f>0.0061988</f>
+        <v>6.1988E-3</v>
+      </c>
+      <c r="K53" s="2">
+        <f>0.0007889</f>
+        <v>7.8890000000000004E-4</v>
+      </c>
+      <c r="L53" s="2">
+        <f>0.004437</f>
+        <v>4.437E-3</v>
+      </c>
+      <c r="M53" s="2">
+        <f>0.000883</f>
+        <v>8.83E-4</v>
+      </c>
+      <c r="N53" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O53" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="2">
+        <f>0.015789</f>
+        <v>1.5789000000000001E-2</v>
+      </c>
+      <c r="C54" s="2">
+        <f>0.002182</f>
+        <v>2.1819999999999999E-3</v>
+      </c>
+      <c r="D54" s="2">
+        <f>0.022441</f>
+        <v>2.2440999999999999E-2</v>
+      </c>
+      <c r="E54" s="2">
+        <f>0.00396</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="F54" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G54" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>52</v>
+      </c>
+      <c r="J54" s="2">
+        <f>0.00843</f>
+        <v>8.43E-3</v>
+      </c>
+      <c r="K54" s="2">
+        <f>0.001284</f>
+        <v>1.284E-3</v>
+      </c>
+      <c r="L54" s="2">
+        <f>0.01068</f>
+        <v>1.068E-2</v>
+      </c>
+      <c r="M54" s="2">
+        <f>0.002145</f>
+        <v>2.1450000000000002E-3</v>
+      </c>
+      <c r="N54" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="O54" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="2">
+        <f>0.089603</f>
+        <v>8.9603000000000002E-2</v>
+      </c>
+      <c r="C55" s="2">
+        <f>0.0137516</f>
+        <v>1.3751599999999999E-2</v>
+      </c>
+      <c r="D55" s="2">
+        <f>0.0739039</f>
+        <v>7.3903899999999995E-2</v>
+      </c>
+      <c r="E55" s="2">
+        <f>0.01291875</f>
+        <v>1.291875E-2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="G55" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>53</v>
+      </c>
+      <c r="J55" s="2">
+        <f>0.0434939</f>
+        <v>4.3493900000000002E-2</v>
+      </c>
+      <c r="K55" s="2">
+        <f>0.005384</f>
+        <v>5.3839999999999999E-3</v>
+      </c>
+      <c r="L55" s="2">
+        <f>0.021504</f>
+        <v>2.1503999999999999E-2</v>
+      </c>
+      <c r="M55" s="2">
+        <f>0.006623</f>
+        <v>6.6230000000000004E-3</v>
+      </c>
+      <c r="N55" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="O55" s="1">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004B8CB5B4B13194088C501F1A73AB836" ma:contentTypeVersion="5" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="6ab33585d7507d8f7d3bdeb41e8bede6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="264d1835de1ad1b918f71464e80c9360" ns3:_="">
     <xsd:import namespace="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa"/>
@@ -3706,6 +4175,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3716,22 +4191,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC555542-73CF-4BDB-AC57-32AF5F06904D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50D3E216-EEFC-4B0C-99CC-A4BBCCB53B96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3749,6 +4208,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC555542-73CF-4BDB-AC57-32AF5F06904D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1ab8b88-ea59-48ac-8d7f-e26084dcc9aa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5C7046A-D9FD-4091-BEF8-46967EC5E81E}">
   <ds:schemaRefs>

</xml_diff>